<commit_message>
Right way eddited xlsx
</commit_message>
<xml_diff>
--- a/src/planilha.xlsx
+++ b/src/planilha.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Documents\Programming\gitViews\trelloToXlsx\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fncosta\Documents\Programming\Python\trelloToXlsx\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E86ED-F3D4-44FD-8B07-B0F94C1BB812}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11217FC-73A2-4E39-ACBE-D10B9E1D1E0A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" tabRatio="402" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="2400" windowWidth="15375" windowHeight="7995" tabRatio="402" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t xml:space="preserve">PRAZOS </t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>OBSERVAÇÕES</t>
-  </si>
-  <si>
-    <t>STATUS</t>
   </si>
   <si>
     <t>PRAZO FATAL</t>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>Recolher custas edital</t>
-  </si>
-  <si>
-    <t>aguardar pagamento</t>
   </si>
   <si>
     <t>0003750-87.2019.8.26.0634</t>
@@ -123,18 +117,21 @@
   <si>
     <t>Vitória Tiannamen</t>
   </si>
+  <si>
+    <t>VITÓRIA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
+    <numFmt numFmtId="6" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
-    <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -240,13 +237,6 @@
       <i/>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -358,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,9 +364,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -413,7 +400,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -427,9 +413,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,9 +444,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -491,19 +471,16 @@
     <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -513,6 +490,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,51 +840,49 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K946"/>
+  <dimension ref="B1:J947"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="35" style="17" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="35" style="16" customWidth="1"/>
     <col min="5" max="5" width="28.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="19" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="9" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="21" customWidth="1"/>
-    <col min="11" max="11" width="12" style="9" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" style="3" customWidth="1"/>
-    <col min="13" max="18" width="9.140625" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="6" width="18.140625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="18" customWidth="1"/>
+    <col min="8" max="8" width="12" style="8" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="12" style="8" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="3" customWidth="1"/>
+    <col min="12" max="17" width="9.140625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="2:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40">
         <v>43882</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="2:11" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="2:10" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14"/>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
@@ -911,234 +895,230 @@
       <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="2:10" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="5">
+        <v>43880</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
-        <v>43880</v>
-      </c>
-      <c r="C4" s="30" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E5" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="G5" s="46"/>
+      <c r="H5" s="25">
+        <v>43892</v>
+      </c>
+      <c r="I5" s="26">
+        <v>43889</v>
+      </c>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="5">
+        <v>43881</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="28">
+      <c r="E6" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="47">
+        <v>451.29</v>
+      </c>
+      <c r="H6" s="25">
+        <v>43893</v>
+      </c>
+      <c r="I6" s="26">
         <v>43892</v>
       </c>
-      <c r="J4" s="29">
-        <v>43889</v>
-      </c>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
-        <v>43881</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="5">
+        <v>43882</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="52">
-        <v>451.29</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="E7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="28">
-        <v>43893</v>
-      </c>
-      <c r="J5" s="29">
-        <v>43892</v>
-      </c>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
-        <v>43882</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <v>43871</v>
+      </c>
+      <c r="C8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="52"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
-        <v>43871</v>
-      </c>
-      <c r="C7" s="30" t="s">
+      <c r="E8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="G8" s="46"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="5">
+        <v>43861</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="5">
-        <v>43861</v>
-      </c>
-      <c r="C8" s="30" t="s">
+      <c r="E9" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="G9" s="46"/>
+      <c r="H9" s="25">
+        <v>43899</v>
+      </c>
+      <c r="I9" s="26">
+        <v>43896</v>
+      </c>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="2:10" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="30">
+        <v>43873</v>
+      </c>
+      <c r="C10" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="11" t="s">
+      <c r="D10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="51"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="28">
+      <c r="E10" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="34"/>
+      <c r="H10" s="37">
+        <v>43900</v>
+      </c>
+      <c r="I10" s="36">
         <v>43899</v>
       </c>
-      <c r="J8" s="29">
-        <v>43896</v>
-      </c>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" spans="2:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
-        <v>43873</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="35" t="s">
+      <c r="J10" s="31"/>
+    </row>
+    <row r="11" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="36" t="s">
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="2:10" s="29" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="30">
+        <v>43815</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="41">
-        <v>43900</v>
-      </c>
-      <c r="J9" s="40">
-        <v>43899</v>
-      </c>
-      <c r="K9" s="34"/>
-    </row>
-    <row r="10" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="43" t="s">
+      <c r="D12" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="2:11" s="32" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33">
-        <v>43815</v>
-      </c>
-      <c r="C11" s="35" t="s">
+      <c r="E12" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="G12" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="36" t="s">
+      <c r="H12" s="35"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="31"/>
+    </row>
+    <row r="13" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="34"/>
-    </row>
-    <row r="12" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="50"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -1152,12 +1132,12 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
-      <c r="C20" s="16" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
+      <c r="C21" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
@@ -3934,12 +3914,15 @@
     <row r="946" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B946" s="3"/>
     </row>
+    <row r="947" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B947" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>